<commit_message>
Fazendo alterações na Apresentação e no Backlog
</commit_message>
<xml_diff>
--- a/projetoCorona/documentação/Backlog.xlsx
+++ b/projetoCorona/documentação/Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Família\Desktop\Minha-Pasta\DigitalSolutions\projetoCorona\documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{602FF667-27E2-4FC4-850D-68A30DBD1F28}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F97B9E0-B69B-48DA-8872-ADD4FF50A195}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{257660E5-54BF-49B4-AC86-9A4BA701822D}"/>
   </bookViews>
@@ -96,20 +96,20 @@
     </r>
   </si>
   <si>
-    <t>Response web</t>
-  </si>
-  <si>
     <t>Computational Thinking  &amp; Domain Driven</t>
   </si>
   <si>
     <t>IA_Chatbots</t>
+  </si>
+  <si>
+    <t>Response Web</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,13 +140,6 @@
     <font>
       <sz val="16"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -205,24 +198,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -539,8 +531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD7E7A49-EA50-43EE-96F6-960DF22F702F}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,204 +544,204 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="1">
         <v>7</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="1">
         <v>16</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="1">
         <v>8</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="1">
         <v>16</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="1">
         <v>8</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="1">
         <v>16</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="1">
         <v>13</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="1">
         <v>12</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="1">
         <v>13</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="1">
         <v>12</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="1">
         <v>13</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="1">
         <v>12</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="1">
+        <v>5</v>
+      </c>
+      <c r="C12" s="1">
+        <v>9</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="1">
+        <v>13</v>
+      </c>
+      <c r="C13" s="1">
+        <v>9</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="4">
-        <v>5</v>
-      </c>
-      <c r="C12" s="4">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="1">
+        <v>13</v>
+      </c>
+      <c r="C15" s="1">
         <v>9</v>
       </c>
-      <c r="D12" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="4">
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="1">
         <v>13</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C17" s="1">
         <v>9</v>
       </c>
-      <c r="D13" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" s="4">
-        <v>13</v>
-      </c>
-      <c r="C15" s="4">
-        <v>9</v>
-      </c>
-      <c r="D15" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="4">
-        <v>13</v>
-      </c>
-      <c r="C17" s="4">
-        <v>9</v>
-      </c>
-      <c r="D17" s="4">
+      <c r="D17" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>